<commit_message>
updated usrep reeds data and finished projections_all_sm
</commit_message>
<xml_diff>
--- a/data-raw/lulucf/lulucf_lts.xlsx
+++ b/data-raw/lulucf/lulucf_lts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlopez\Github\BTR\data-raw\lulucf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\BTR\data-raw\lulucf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437A4D0E-E484-41DF-B420-C3596EF56087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BFA410-885B-4A0C-B7E6-1F3B1304259F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{420A80F6-E1CF-424D-9063-F8EC805B5804}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="18900" windowHeight="10890" xr2:uid="{420A80F6-E1CF-424D-9063-F8EC805B5804}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="15">
   <si>
     <t>scenario</t>
   </si>
@@ -432,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84AD23CA-48B7-40FD-A38E-7A45F51157BF}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,6 +446,7 @@
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -479,7 +480,7 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="D2">
         <v>-743.09711157562333</v>
@@ -502,10 +503,10 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="D3">
-        <v>-659.26322942720196</v>
+        <v>-743.09711157562333</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -525,10 +526,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="D4">
-        <v>-554.02036161887133</v>
+        <v>-659.26322942720196</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -548,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="D5">
-        <v>-509.18138093476944</v>
+        <v>-554.02036161887133</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -571,10 +572,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>2050</v>
+        <v>2045</v>
       </c>
       <c r="D6">
-        <v>-475.75686480370655</v>
+        <v>-509.18138093476944</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -591,13 +592,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>2019</v>
+        <v>2050</v>
       </c>
       <c r="D7">
-        <v>-812.7</v>
+        <v>-475.75686480370655</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -617,10 +618,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="D8">
-        <v>-883.90327395269583</v>
+        <v>-743.09711157562333</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -640,10 +641,10 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="D9">
-        <v>-952.20654790539174</v>
+        <v>-883.90327395269583</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -663,10 +664,10 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="D10">
-        <v>-989.30734376972725</v>
+        <v>-952.20654790539174</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -686,10 +687,10 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="D11">
-        <v>-1026.4081396340628</v>
+        <v>-989.30734376972725</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -709,10 +710,10 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>2050</v>
+        <v>2045</v>
       </c>
       <c r="D12">
-        <v>-1063.5089354983984</v>
+        <v>-1026.4081396340628</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -729,13 +730,13 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="D13">
-        <v>-834.16236046451206</v>
+        <v>-1063.5089354983984</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -755,10 +756,10 @@
         <v>11</v>
       </c>
       <c r="C14">
-        <v>2035</v>
+        <v>2025</v>
       </c>
       <c r="D14">
-        <v>-782.87394609386831</v>
+        <v>-834.16236046451206</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
@@ -778,10 +779,10 @@
         <v>11</v>
       </c>
       <c r="C15">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="D15">
-        <v>-708.83046661887136</v>
+        <v>-834.16236046451206</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -801,10 +802,10 @@
         <v>11</v>
       </c>
       <c r="C16">
-        <v>2045</v>
+        <v>2035</v>
       </c>
       <c r="D16">
-        <v>-667.73587426810309</v>
+        <v>-782.87394609386831</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -824,10 +825,10 @@
         <v>11</v>
       </c>
       <c r="C17">
-        <v>2050</v>
+        <v>2040</v>
       </c>
       <c r="D17">
-        <v>-636.39865194656397</v>
+        <v>-708.83046661887136</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
@@ -844,13 +845,13 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>2030</v>
+        <v>2045</v>
       </c>
       <c r="D18">
-        <v>-1041.8755864526959</v>
+        <v>-667.73587426810309</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -867,13 +868,13 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19">
-        <v>2035</v>
+        <v>2050</v>
       </c>
       <c r="D19">
-        <v>-1166.566857905392</v>
+        <v>-636.39865194656397</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -893,10 +894,10 @@
         <v>12</v>
       </c>
       <c r="C20">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="D20">
-        <v>-1261.1472212697272</v>
+        <v>-1041.8755864526959</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -916,10 +917,10 @@
         <v>12</v>
       </c>
       <c r="C21">
-        <v>2045</v>
+        <v>2030</v>
       </c>
       <c r="D21">
-        <v>-1318.0142513007293</v>
+        <v>-1041.8755864526959</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -939,18 +940,87 @@
         <v>12</v>
       </c>
       <c r="C22">
+        <v>2035</v>
+      </c>
+      <c r="D22">
+        <v>-1166.566857905392</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>2040</v>
+      </c>
+      <c r="D23">
+        <v>-1261.1472212697272</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>2045</v>
+      </c>
+      <c r="D24">
+        <v>-1318.0142513007293</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25">
         <v>2050</v>
       </c>
-      <c r="D22">
+      <c r="D25">
         <v>-1352.8343715698268</v>
       </c>
-      <c r="E22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>